<commit_message>
antes de cargar datos reales fer
</commit_message>
<xml_diff>
--- a/Basededatos/detalles_transformadores.xlsx
+++ b/Basededatos/detalles_transformadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B62691C-0D01-467A-A67E-B758A3C6695C}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5439D8-FD30-4BB1-9159-A83AF5F8AB0C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11242185-241D-4A74-AA8F-D46A2BE7D9FB}"/>
   </bookViews>
@@ -2157,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1F543B-E208-4497-A3ED-9DFED7C26A7E}">
   <dimension ref="A1:M167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="L142" sqref="L142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5835,7 +5835,7 @@
         <v>200</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>194</v>
+        <v>86</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>320</v>
@@ -5907,7 +5907,7 @@
         <v>40</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>11</v>
@@ -5946,7 +5946,7 @@
         <v>41</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>11</v>
@@ -5985,7 +5985,7 @@
         <v>42</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>11</v>
@@ -6024,7 +6024,7 @@
         <v>175</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>320</v>
@@ -14680,15 +14680,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100973BFEFB9E8EED45AA48D1DFC8B704A3" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="48fa98e84d6ca432d9ec38d9b25c34f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8208d0d75ea2fc72020bc14120e8df3f" ns3:_="">
     <xsd:import namespace="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
@@ -14870,6 +14861,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -14879,14 +14879,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C89EA1E5-D714-4CF4-A402-332B720743E2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14904,18 +14896,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB6E9F9-7002-453D-A23F-C770D0B18A16}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
antes de borrar los datos aleatorios de oltc,furanos,rnuc
</commit_message>
<xml_diff>
--- a/Basededatos/detalles_transformadores.xlsx
+++ b/Basededatos/detalles_transformadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5439D8-FD30-4BB1-9159-A83AF5F8AB0C}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDADB7D0-DE33-4BCA-BFE1-535420216CC1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11242185-241D-4A74-AA8F-D46A2BE7D9FB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2863" uniqueCount="353">
   <si>
     <t>Alto Pradera</t>
   </si>
@@ -1082,6 +1082,15 @@
   </si>
   <si>
     <t>40</t>
+  </si>
+  <si>
+    <t>348447</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1292,6 +1301,12 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1834,10 +1849,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}" name="Tabla1" displayName="Tabla1" ref="A1:M167" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:M167" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}"/>
-  <sortState ref="A2:E166">
-    <sortCondition ref="B2:B166"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}" name="Tabla1" displayName="Tabla1" ref="A1:M168" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:M168" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}"/>
+  <sortState ref="A2:E167">
+    <sortCondition ref="B2:B167"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{F6344666-3F16-4B8F-9819-0B63A270CC95}" name="SERIE" dataDxfId="12" dataCellStyle="Normal 2"/>
@@ -2155,10 +2170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1F543B-E208-4497-A3ED-9DFED7C26A7E}">
-  <dimension ref="A1:M167"/>
+  <dimension ref="A1:M168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="L142" sqref="L142"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6904,47 +6919,33 @@
       <c r="M127" s="10"/>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A128" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B128" s="15" t="s">
-        <v>8</v>
+      <c r="A128" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>7</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D128" s="1"/>
       <c r="E128" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F128" s="1">
-        <v>80</v>
-      </c>
-      <c r="G128" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="H128" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="I128" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="J128" s="5">
-        <v>2016</v>
+        <v>351</v>
+      </c>
+      <c r="F128" s="1"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="5"/>
+      <c r="J128" s="5" t="s">
+        <v>352</v>
       </c>
       <c r="K128" s="5"/>
-      <c r="L128" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="M128" s="10" t="s">
-        <v>332</v>
-      </c>
+      <c r="L128" s="5"/>
+      <c r="M128" s="10"/>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B129" s="15" t="s">
         <v>8</v>
@@ -6953,7 +6954,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>58</v>
@@ -6983,7 +6984,7 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B130" s="15" t="s">
         <v>8</v>
@@ -6992,7 +6993,7 @@
         <v>11</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>58</v>
@@ -7022,16 +7023,16 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B131" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>58</v>
@@ -7049,11 +7050,11 @@
         <v>212</v>
       </c>
       <c r="J131" s="5">
-        <v>2023</v>
+        <v>2016</v>
       </c>
       <c r="K131" s="5"/>
       <c r="L131" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M131" s="10" t="s">
         <v>332</v>
@@ -7061,7 +7062,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B132" s="15" t="s">
         <v>8</v>
@@ -7070,7 +7071,7 @@
         <v>13</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>58</v>
@@ -7100,7 +7101,7 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B133" s="15" t="s">
         <v>8</v>
@@ -7109,7 +7110,7 @@
         <v>13</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>58</v>
@@ -7139,153 +7140,153 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B134" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B134" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D134" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E134" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F134" s="1">
-        <v>50</v>
-      </c>
-      <c r="G134" s="5">
-        <v>50</v>
+        <v>80</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="I134" s="5" t="s">
         <v>212</v>
       </c>
       <c r="J134" s="5">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="K134" s="5"/>
       <c r="L134" s="5" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="M134" s="10" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B135" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B135" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>320</v>
+        <v>12</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="5" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="F135" s="1">
-        <v>80</v>
-      </c>
-      <c r="G135" s="5" t="s">
-        <v>296</v>
+        <v>50</v>
+      </c>
+      <c r="G135" s="5">
+        <v>50</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="I135" s="5" t="s">
         <v>212</v>
       </c>
       <c r="J135" s="5">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="K135" s="5"/>
-      <c r="L135" s="5"/>
-      <c r="M135" s="10"/>
+      <c r="L135" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="M135" s="10" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="B136" s="15" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>99</v>
+        <v>320</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="5" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="F136" s="1">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>278</v>
+        <v>227</v>
       </c>
       <c r="I136" s="5" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="J136" s="5">
-        <v>1998</v>
+        <v>2017</v>
       </c>
       <c r="K136" s="5"/>
-      <c r="L136" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="M136" s="10" t="s">
-        <v>329</v>
-      </c>
+      <c r="L136" s="5"/>
+      <c r="M136" s="10"/>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="B137" s="15" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D137" s="1"/>
       <c r="E137" s="5" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="F137" s="1">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>210</v>
+        <v>277</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>227</v>
+        <v>278</v>
       </c>
       <c r="I137" s="5" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="J137" s="5">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="K137" s="5"/>
       <c r="L137" s="5" t="s">
         <v>323</v>
       </c>
       <c r="M137" s="10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B138" s="15" t="s">
         <v>9</v>
@@ -7294,7 +7295,7 @@
         <v>12</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>58</v>
@@ -7324,7 +7325,7 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B139" s="15" t="s">
         <v>9</v>
@@ -7333,7 +7334,7 @@
         <v>12</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>58</v>
@@ -7363,26 +7364,28 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B140" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D140" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E140" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F140" s="1">
-        <v>50</v>
-      </c>
-      <c r="G140" s="5">
-        <v>50</v>
+        <v>80</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I140" s="5" t="s">
         <v>228</v>
@@ -7395,45 +7398,49 @@
         <v>323</v>
       </c>
       <c r="M140" s="10" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="B141" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>320</v>
+        <v>13</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F141" s="1">
-        <v>80</v>
-      </c>
-      <c r="G141" s="5" t="s">
-        <v>296</v>
+        <v>50</v>
+      </c>
+      <c r="G141" s="5">
+        <v>50</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="I141" s="5" t="s">
         <v>228</v>
       </c>
       <c r="J141" s="5">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="K141" s="5"/>
-      <c r="L141" s="5"/>
-      <c r="M141" s="10"/>
+      <c r="L141" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="M141" s="10" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B142" s="15" t="s">
         <v>9</v>
@@ -7443,16 +7450,16 @@
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F142" s="1">
-        <v>50</v>
-      </c>
-      <c r="G142" s="5">
-        <v>50</v>
+        <v>80</v>
+      </c>
+      <c r="G142" s="5" t="s">
+        <v>296</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>297</v>
+        <v>211</v>
       </c>
       <c r="I142" s="5" t="s">
         <v>228</v>
@@ -7466,69 +7473,65 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>99</v>
+        <v>320</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="5" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="F143" s="1">
-        <v>25</v>
-      </c>
-      <c r="G143" s="5" t="s">
-        <v>242</v>
+        <v>50</v>
+      </c>
+      <c r="G143" s="5">
+        <v>50</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="I143" s="5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="J143" s="5">
-        <v>1995</v>
+        <v>2018</v>
       </c>
       <c r="K143" s="5"/>
-      <c r="L143" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="M143" s="10">
-        <v>65.344999999999999</v>
-      </c>
+      <c r="L143" s="5"/>
+      <c r="M143" s="10"/>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A144" s="8">
-        <v>147400</v>
+      <c r="A144" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="B144" s="15" t="s">
         <v>92</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F144" s="1">
         <v>25</v>
       </c>
       <c r="G144" s="5" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="I144" s="5" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="J144" s="5">
-        <v>2016</v>
+        <v>1995</v>
       </c>
       <c r="K144" s="5"/>
       <c r="L144" s="5" t="s">
@@ -7539,33 +7542,33 @@
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A145" s="8" t="s">
-        <v>149</v>
+      <c r="A145" s="8">
+        <v>147400</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F145" s="1">
-        <v>50</v>
-      </c>
-      <c r="G145" s="5">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="G145" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I145" s="5" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="J145" s="5">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="K145" s="5"/>
       <c r="L145" s="5" t="s">
@@ -7576,33 +7579,33 @@
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A146" s="8">
-        <v>146918</v>
+      <c r="A146" s="8" t="s">
+        <v>149</v>
       </c>
       <c r="B146" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F146" s="1">
         <v>50</v>
       </c>
-      <c r="G146" s="5" t="s">
-        <v>238</v>
+      <c r="G146" s="5">
+        <v>50</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="I146" s="5" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="J146" s="5">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="K146" s="5"/>
       <c r="L146" s="5" t="s">
@@ -7613,105 +7616,105 @@
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A147" s="8" t="s">
-        <v>189</v>
+      <c r="A147" s="8">
+        <v>146918</v>
       </c>
       <c r="B147" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>320</v>
+        <v>100</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="5" t="s">
         <v>162</v>
       </c>
       <c r="F147" s="1">
-        <v>25</v>
-      </c>
-      <c r="G147" s="5">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="G147" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>304</v>
+        <v>240</v>
       </c>
       <c r="I147" s="5" t="s">
-        <v>305</v>
+        <v>241</v>
       </c>
       <c r="J147" s="5">
-        <v>1965</v>
+        <v>2014</v>
       </c>
       <c r="K147" s="5"/>
       <c r="L147" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M147" s="10"/>
+      <c r="M147" s="10">
+        <v>65.344999999999999</v>
+      </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>150</v>
+        <v>189</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>99</v>
+        <v>320</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F148" s="1">
-        <v>50</v>
-      </c>
-      <c r="G148" s="5" t="s">
-        <v>238</v>
+        <v>25</v>
+      </c>
+      <c r="G148" s="5">
+        <v>25</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
       <c r="I148" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="J148" s="5" t="s">
-        <v>279</v>
+        <v>305</v>
+      </c>
+      <c r="J148" s="5">
+        <v>1965</v>
       </c>
       <c r="K148" s="5"/>
       <c r="L148" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M148" s="10">
-        <v>65.344999999999999</v>
-      </c>
+      <c r="M148" s="10"/>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B149" s="15" t="s">
         <v>94</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F149" s="1">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I149" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="J149" s="5">
-        <v>1995</v>
+        <v>245</v>
+      </c>
+      <c r="J149" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="K149" s="5"/>
       <c r="L149" s="5" t="s">
@@ -7723,81 +7726,79 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B150" s="15" t="s">
         <v>94</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>320</v>
+        <v>100</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="5" t="s">
         <v>162</v>
       </c>
       <c r="F150" s="1">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="G150" s="5" t="s">
-        <v>306</v>
+        <v>242</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>307</v>
+        <v>258</v>
       </c>
       <c r="I150" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="J150" s="5" t="s">
-        <v>308</v>
+        <v>225</v>
+      </c>
+      <c r="J150" s="5">
+        <v>1995</v>
       </c>
       <c r="K150" s="5"/>
       <c r="L150" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M150" s="10"/>
+      <c r="M150" s="10">
+        <v>65.344999999999999</v>
+      </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B151" s="17" t="s">
-        <v>10</v>
+        <v>190</v>
+      </c>
+      <c r="B151" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="D151" s="1"/>
       <c r="E151" s="5" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="F151" s="1">
-        <v>40</v>
+        <v>12.5</v>
       </c>
       <c r="G151" s="5" t="s">
-        <v>218</v>
+        <v>306</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>224</v>
+        <v>307</v>
       </c>
       <c r="I151" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="J151" s="5">
-        <v>1998</v>
+        <v>247</v>
+      </c>
+      <c r="J151" s="5" t="s">
+        <v>308</v>
       </c>
       <c r="K151" s="5"/>
       <c r="L151" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="M151" s="10" t="s">
-        <v>334</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="M151" s="10"/>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B152" s="17" t="s">
         <v>10</v>
@@ -7806,7 +7807,7 @@
         <v>13</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E152" s="5" t="s">
         <v>58</v>
@@ -7836,7 +7837,7 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B153" s="17" t="s">
         <v>10</v>
@@ -7845,7 +7846,7 @@
         <v>13</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E153" s="5" t="s">
         <v>58</v>
@@ -7860,10 +7861,10 @@
         <v>224</v>
       </c>
       <c r="I153" s="5" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="J153" s="5">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="K153" s="5"/>
       <c r="L153" s="5" t="s">
@@ -7875,16 +7876,16 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
-        <v>340</v>
+        <v>57</v>
       </c>
       <c r="B154" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E154" s="5" t="s">
         <v>58</v>
@@ -7896,25 +7897,25 @@
         <v>218</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="I154" s="5" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="J154" s="5">
-        <v>1996</v>
+        <v>2017</v>
       </c>
       <c r="K154" s="5"/>
       <c r="L154" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M154" s="10" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A155" s="8">
-        <v>59572</v>
+      <c r="A155" s="8" t="s">
+        <v>340</v>
       </c>
       <c r="B155" s="17" t="s">
         <v>10</v>
@@ -7923,7 +7924,7 @@
         <v>14</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E155" s="5" t="s">
         <v>58</v>
@@ -7953,7 +7954,7 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="8">
-        <v>59573</v>
+        <v>59572</v>
       </c>
       <c r="B156" s="17" t="s">
         <v>10</v>
@@ -7962,7 +7963,7 @@
         <v>14</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E156" s="5" t="s">
         <v>58</v>
@@ -7991,16 +7992,18 @@
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A157" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B157" s="15" t="s">
+      <c r="A157" s="8">
+        <v>59573</v>
+      </c>
+      <c r="B157" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D157" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E157" s="5" t="s">
         <v>58</v>
       </c>
@@ -8008,66 +8011,64 @@
         <v>40</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="I157" s="5" t="s">
         <v>225</v>
       </c>
       <c r="J157" s="5">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="K157" s="5"/>
-      <c r="L157" s="5"/>
-      <c r="M157" s="10"/>
+      <c r="L157" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="M157" s="10" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="B158" s="15" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>99</v>
+        <v>320</v>
       </c>
       <c r="D158" s="1"/>
       <c r="E158" s="5" t="s">
-        <v>162</v>
+        <v>58</v>
       </c>
       <c r="F158" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G158" s="5" t="s">
-        <v>280</v>
+        <v>223</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>281</v>
+        <v>224</v>
       </c>
       <c r="I158" s="5" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
       <c r="J158" s="5">
-        <v>1966</v>
-      </c>
-      <c r="K158" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="L158" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="M158" s="10">
-        <v>65.344999999999999</v>
-      </c>
+        <v>1998</v>
+      </c>
+      <c r="K158" s="5"/>
+      <c r="L158" s="5"/>
+      <c r="M158" s="10"/>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B159" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>99</v>
@@ -8077,22 +8078,22 @@
         <v>162</v>
       </c>
       <c r="F159" s="1">
-        <v>50</v>
-      </c>
-      <c r="G159" s="5">
-        <v>50</v>
+        <v>5</v>
+      </c>
+      <c r="G159" s="5" t="s">
+        <v>280</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="I159" s="5" t="s">
-        <v>241</v>
+        <v>282</v>
       </c>
       <c r="J159" s="5">
-        <v>2018</v>
+        <v>1966</v>
       </c>
       <c r="K159" s="5" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="L159" s="5" t="s">
         <v>323</v>
@@ -8103,35 +8104,35 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B160" s="15" t="s">
         <v>96</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D160" s="1"/>
       <c r="E160" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F160" s="1">
-        <v>25</v>
-      </c>
-      <c r="G160" s="5" t="s">
-        <v>283</v>
+        <v>50</v>
+      </c>
+      <c r="G160" s="5">
+        <v>50</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="I160" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="J160" s="5" t="s">
-        <v>284</v>
+        <v>241</v>
+      </c>
+      <c r="J160" s="5">
+        <v>2018</v>
       </c>
       <c r="K160" s="5" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="L160" s="5" t="s">
         <v>323</v>
@@ -8142,32 +8143,32 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B161" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F161" s="1">
         <v>25</v>
       </c>
       <c r="G161" s="5" t="s">
-        <v>242</v>
+        <v>283</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="I161" s="5" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="J161" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K161" s="5" t="s">
         <v>345</v>
@@ -8181,13 +8182,13 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B162" s="15" t="s">
         <v>97</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="5" t="s">
@@ -8196,17 +8197,17 @@
       <c r="F162" s="1">
         <v>25</v>
       </c>
-      <c r="G162" s="5">
-        <v>25</v>
+      <c r="G162" s="5" t="s">
+        <v>242</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
       <c r="I162" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="J162" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K162" s="5" t="s">
         <v>345</v>
@@ -8220,13 +8221,13 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="B163" s="15" t="s">
         <v>97</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>320</v>
+        <v>100</v>
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="5" t="s">
@@ -8235,33 +8236,37 @@
       <c r="F163" s="1">
         <v>25</v>
       </c>
-      <c r="G163" s="5" t="s">
-        <v>242</v>
+      <c r="G163" s="5">
+        <v>25</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="I163" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="J163" s="5">
-        <v>1980</v>
-      </c>
-      <c r="K163" s="5"/>
+        <v>245</v>
+      </c>
+      <c r="J163" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="K163" s="5" t="s">
+        <v>345</v>
+      </c>
       <c r="L163" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M163" s="10"/>
+      <c r="M163" s="10">
+        <v>65.344999999999999</v>
+      </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="B164" s="15" t="s">
-        <v>288</v>
+        <v>97</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>99</v>
+        <v>320</v>
       </c>
       <c r="D164" s="1"/>
       <c r="E164" s="5" t="s">
@@ -8274,55 +8279,51 @@
         <v>242</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="J164" s="5">
-        <v>1993</v>
-      </c>
-      <c r="K164" s="5" t="s">
-        <v>345</v>
-      </c>
+        <v>1980</v>
+      </c>
+      <c r="K164" s="5"/>
       <c r="L164" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M164" s="10">
-        <v>65.344999999999999</v>
-      </c>
+      <c r="M164" s="10"/>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B165" s="15" t="s">
         <v>288</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F165" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G165" s="5" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="I165" s="5" t="s">
         <v>225</v>
       </c>
       <c r="J165" s="5">
-        <v>2005</v>
+        <v>1993</v>
       </c>
       <c r="K165" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="L165" s="5" t="s">
         <v>323</v>
@@ -8332,76 +8333,115 @@
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A166" s="11" t="s">
+      <c r="A166" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B166" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D166" s="1"/>
+      <c r="E166" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F166" s="1">
+        <v>40</v>
+      </c>
+      <c r="G166" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I166" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="J166" s="5">
+        <v>2005</v>
+      </c>
+      <c r="K166" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="L166" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="M166" s="10">
+        <v>65.344999999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A167" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B166" s="16" t="s">
+      <c r="B167" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="C166" s="13" t="s">
+      <c r="C167" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="D166" s="13"/>
-      <c r="E166" s="12" t="s">
+      <c r="D167" s="13"/>
+      <c r="E167" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="F166" s="13">
+      <c r="F167" s="13">
         <v>25</v>
       </c>
-      <c r="G166" s="12" t="s">
+      <c r="G167" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="H166" s="13" t="s">
+      <c r="H167" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="I166" s="12" t="s">
+      <c r="I167" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="J166" s="12">
+      <c r="J167" s="12">
         <v>1980</v>
       </c>
-      <c r="K166" s="12"/>
-      <c r="L166" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="M166" s="14"/>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
+      <c r="K167" s="12"/>
+      <c r="L167" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="M167" s="14"/>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B167" s="15" t="s">
+      <c r="B168" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="C168" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D167" s="1"/>
-      <c r="E167" s="5" t="s">
+      <c r="D168" s="1"/>
+      <c r="E168" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="F167" s="1">
+      <c r="F168" s="1">
         <v>25</v>
       </c>
-      <c r="G167" s="5" t="s">
+      <c r="G168" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="H167" s="1" t="s">
+      <c r="H168" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="I167" s="5" t="s">
+      <c r="I168" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="J167" s="5" t="s">
+      <c r="J168" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="K167" s="5" t="s">
+      <c r="K168" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="L167" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="M167" s="5">
+      <c r="L168" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="M168" s="5">
         <v>65.344999999999999</v>
       </c>
     </row>
@@ -14680,6 +14720,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100973BFEFB9E8EED45AA48D1DFC8B704A3" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="48fa98e84d6ca432d9ec38d9b25c34f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8208d0d75ea2fc72020bc14120e8df3f" ns3:_="">
     <xsd:import namespace="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
@@ -14861,15 +14910,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -14879,6 +14919,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C89EA1E5-D714-4CF4-A402-332B720743E2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14896,26 +14944,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB6E9F9-7002-453D-A23F-C770D0B18A16}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
actualizado con datos reales antes de hacer pruebas machine learning con DGA
</commit_message>
<xml_diff>
--- a/Basededatos/detalles_transformadores.xlsx
+++ b/Basededatos/detalles_transformadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDADB7D0-DE33-4BCA-BFE1-535420216CC1}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{A918A0E3-CE11-49BB-820A-1F2C589F71AA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11242185-241D-4A74-AA8F-D46A2BE7D9FB}"/>
   </bookViews>
@@ -2172,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1F543B-E208-4497-A3ED-9DFED7C26A7E}">
   <dimension ref="A1:M168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14720,12 +14720,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14911,17 +14910,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB6E9F9-7002-453D-A23F-C770D0B18A16}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14945,17 +14953,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB6E9F9-7002-453D-A23F-C770D0B18A16}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
se optimizó código hi,ais,arr,bus,nuc y se avanzó Vida Utilizada
</commit_message>
<xml_diff>
--- a/Basededatos/detalles_transformadores.xlsx
+++ b/Basededatos/detalles_transformadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECD38895-F506-416A-A86D-9E13A8B0A9C8}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="6_{F1E03C79-CB95-42C2-A5F2-68DAEC76D33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BA053E2-1D7C-45FE-AFB0-2B3EC43708F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11242185-241D-4A74-AA8F-D46A2BE7D9FB}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2864" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2992" uniqueCount="361">
   <si>
     <t>SERIE</t>
   </si>
@@ -1091,6 +1091,27 @@
   </si>
   <si>
     <t>146660T3(ANTES)</t>
+  </si>
+  <si>
+    <t>Tres Hermanas</t>
+  </si>
+  <si>
+    <t>130393A/01</t>
+  </si>
+  <si>
+    <t>140515A/01</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>Termoestabilizado</t>
+  </si>
+  <si>
+    <t>Kraft</t>
+  </si>
+  <si>
+    <t>No-Termoestabilizado</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1162,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1160,8 +1181,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1265,12 +1292,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1307,12 +1347,60 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{3014A368-80E9-4EAB-913F-5CFA4FBE9311}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1849,22 +1937,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}" name="Tabla1" displayName="Tabla1" ref="A1:M169" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:M169" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F6344666-3F16-4B8F-9819-0B63A270CC95}" name="SERIE" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{BF3A1E42-E0D9-4CDF-8A8F-4D01DA9C2734}" name="SUBESTACION" dataDxfId="11" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{086311AC-BD2B-4D39-A59F-C2F3DBB5BD0F}" name="CIRCUITO" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{757AE7E8-24CE-4AA1-8778-20FAE11E45E5}" name="FASE" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{D454E399-B0D4-42AB-9912-282FD4830B8E}" name="TENSION" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{3CC8E47F-98F3-4318-AB1D-FAC9E7BC6874}" name="POT. INSTALADA" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{23F07AF9-B84D-4BF9-9DF2-DE1D85185F50}" name="POT. PLACA" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{ED7CF816-59D2-4619-8E39-1E2BDCA457A2}" name="RELACION TRANSFORMACION" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{CEE0FEA8-A128-445D-BD33-1D7629A44FBD}" name="MARCA" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{5E1DA30F-CECE-4D50-ACC9-1667500CE4C8}" name="Año Fab." dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{AB2BEE58-DAE3-42F4-9462-6851FF1D161C}" name="POTENCIA" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{DABF4449-1876-463F-885E-3BF16AA12BAF}" name="POS. TAP" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{3C994351-839D-4BCF-BCD5-B289A1CC0FEA}" name="TENSION TAP" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}" name="Tabla1" displayName="Tabla1" ref="A1:N171" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:N171" xr:uid="{5F56859F-08D4-4BC2-887B-4FF00B101B3E}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{F6344666-3F16-4B8F-9819-0B63A270CC95}" name="SERIE" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{BF3A1E42-E0D9-4CDF-8A8F-4D01DA9C2734}" name="SUBESTACION" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{086311AC-BD2B-4D39-A59F-C2F3DBB5BD0F}" name="CIRCUITO" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{757AE7E8-24CE-4AA1-8778-20FAE11E45E5}" name="FASE" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{D454E399-B0D4-42AB-9912-282FD4830B8E}" name="TENSION" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3CC8E47F-98F3-4318-AB1D-FAC9E7BC6874}" name="POT. INSTALADA" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{23F07AF9-B84D-4BF9-9DF2-DE1D85185F50}" name="POT. PLACA" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{ED7CF816-59D2-4619-8E39-1E2BDCA457A2}" name="RELACION TRANSFORMACION" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{CEE0FEA8-A128-445D-BD33-1D7629A44FBD}" name="MARCA" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{5E1DA30F-CECE-4D50-ACC9-1667500CE4C8}" name="Año Fab." dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{AB2BEE58-DAE3-42F4-9462-6851FF1D161C}" name="POTENCIA" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{DABF4449-1876-463F-885E-3BF16AA12BAF}" name="POS. TAP" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{3C994351-839D-4BCF-BCD5-B289A1CC0FEA}" name="TENSION TAP" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{2E20140B-2F1F-488C-AA00-B1B7F4224BC0}" name="TIPO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2167,10 +2256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1F543B-E208-4497-A3ED-9DFED7C26A7E}">
-  <dimension ref="A1:M169"/>
+  <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,9 +2277,10 @@
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2230,8 +2320,11 @@
       <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="28" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -2271,8 +2364,11 @@
       <c r="M2" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="27" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -2312,8 +2408,11 @@
       <c r="M3" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
@@ -2353,8 +2452,11 @@
       <c r="M4" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
@@ -2392,8 +2494,11 @@
       <c r="M5" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>34</v>
       </c>
@@ -2425,8 +2530,11 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
@@ -2466,8 +2574,11 @@
       <c r="M7" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>551875</v>
       </c>
@@ -2507,8 +2618,11 @@
       <c r="M8" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>551874</v>
       </c>
@@ -2548,8 +2662,11 @@
       <c r="M9" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -2581,8 +2698,11 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>46</v>
       </c>
@@ -2616,8 +2736,11 @@
         <v>33</v>
       </c>
       <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>51</v>
       </c>
@@ -2655,8 +2778,11 @@
       <c r="M12" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -2694,8 +2820,11 @@
       <c r="M13" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>57</v>
       </c>
@@ -2733,8 +2862,11 @@
       <c r="M14" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
@@ -2772,8 +2904,11 @@
       <c r="M15" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>185635</v>
       </c>
@@ -2811,8 +2946,11 @@
       <c r="M16" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>185636</v>
       </c>
@@ -2850,8 +2988,11 @@
       <c r="M17" s="10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>64</v>
       </c>
@@ -2889,8 +3030,11 @@
       <c r="M18" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>66</v>
       </c>
@@ -2928,8 +3072,11 @@
       <c r="M19" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>67</v>
       </c>
@@ -2967,8 +3114,11 @@
       <c r="M20" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>68</v>
       </c>
@@ -3006,8 +3156,11 @@
       <c r="M21" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>70</v>
       </c>
@@ -3045,8 +3198,11 @@
       <c r="M22" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>71</v>
       </c>
@@ -3084,8 +3240,11 @@
       <c r="M23" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>72</v>
       </c>
@@ -3121,8 +3280,11 @@
       <c r="M24" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>77</v>
       </c>
@@ -3158,8 +3320,11 @@
       <c r="M25" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>364072</v>
       </c>
@@ -3195,8 +3360,11 @@
       <c r="M26" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>83</v>
       </c>
@@ -3234,8 +3402,11 @@
       <c r="M27" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>89</v>
       </c>
@@ -3273,8 +3444,11 @@
       <c r="M28" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>90</v>
       </c>
@@ -3312,8 +3486,11 @@
       <c r="M29" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>91</v>
       </c>
@@ -3345,8 +3522,11 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="10"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>94</v>
       </c>
@@ -3378,8 +3558,11 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="10"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>96</v>
       </c>
@@ -3415,8 +3598,11 @@
       <c r="M32" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>99</v>
       </c>
@@ -3452,8 +3638,11 @@
       <c r="M33" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>103</v>
       </c>
@@ -3489,8 +3678,11 @@
       <c r="M34" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>106</v>
       </c>
@@ -3526,8 +3718,11 @@
       <c r="M35" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>110</v>
       </c>
@@ -3563,8 +3758,11 @@
       <c r="M36" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>115</v>
       </c>
@@ -3598,8 +3796,11 @@
         <v>33</v>
       </c>
       <c r="M37" s="10"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>118</v>
       </c>
@@ -3633,8 +3834,11 @@
         <v>33</v>
       </c>
       <c r="M38" s="10"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>121</v>
       </c>
@@ -3670,8 +3874,11 @@
       <c r="M39" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>127</v>
       </c>
@@ -3707,8 +3914,11 @@
       <c r="M40" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>128</v>
       </c>
@@ -3744,8 +3954,11 @@
       <c r="M41" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>146916</v>
       </c>
@@ -3781,8 +3994,11 @@
       <c r="M42" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>130</v>
       </c>
@@ -3818,8 +4034,11 @@
       <c r="M43" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>132</v>
       </c>
@@ -3857,8 +4076,11 @@
       <c r="M44" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>134</v>
       </c>
@@ -3896,8 +4118,11 @@
       <c r="M45" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>135</v>
       </c>
@@ -3935,8 +4160,11 @@
       <c r="M46" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>185466</v>
       </c>
@@ -3972,8 +4200,11 @@
       <c r="M47" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>137</v>
       </c>
@@ -4009,8 +4240,11 @@
       <c r="M48" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>139</v>
       </c>
@@ -4042,8 +4276,11 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
       <c r="M49" s="10"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>141</v>
       </c>
@@ -4077,8 +4314,11 @@
         <v>33</v>
       </c>
       <c r="M50" s="10"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>142</v>
       </c>
@@ -4114,8 +4354,11 @@
       <c r="M51" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>144</v>
       </c>
@@ -4151,8 +4394,11 @@
       <c r="M52" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>145</v>
       </c>
@@ -4188,8 +4434,11 @@
       <c r="M53" s="10" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>150</v>
       </c>
@@ -4225,8 +4474,11 @@
       <c r="M54" s="10" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>152</v>
       </c>
@@ -4260,8 +4512,11 @@
         <v>33</v>
       </c>
       <c r="M55" s="10"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>154</v>
       </c>
@@ -4295,8 +4550,11 @@
         <v>33</v>
       </c>
       <c r="M56" s="10"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>158</v>
       </c>
@@ -4330,8 +4588,11 @@
         <v>33</v>
       </c>
       <c r="M57" s="10"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>359111</v>
       </c>
@@ -4367,8 +4628,11 @@
       <c r="M58" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>161</v>
       </c>
@@ -4404,8 +4668,11 @@
       <c r="M59" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>165</v>
       </c>
@@ -4441,8 +4708,11 @@
       <c r="M60" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>168</v>
       </c>
@@ -4476,8 +4746,11 @@
         <v>33</v>
       </c>
       <c r="M61" s="10"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>171</v>
       </c>
@@ -4511,8 +4784,11 @@
         <v>33</v>
       </c>
       <c r="M62" s="10"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>173</v>
       </c>
@@ -4546,8 +4822,11 @@
         <v>33</v>
       </c>
       <c r="M63" s="10"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>364074</v>
       </c>
@@ -4583,8 +4862,11 @@
       <c r="M64" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>146917</v>
       </c>
@@ -4620,8 +4902,11 @@
       <c r="M65" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>176</v>
       </c>
@@ -4659,8 +4944,11 @@
       <c r="M66" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>179</v>
       </c>
@@ -4698,8 +4986,11 @@
       <c r="M67" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>180</v>
       </c>
@@ -4737,8 +5028,11 @@
       <c r="M68" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>181</v>
       </c>
@@ -4770,8 +5064,11 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
       <c r="M69" s="10"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>183</v>
       </c>
@@ -4807,8 +5104,11 @@
       <c r="M70" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>186</v>
       </c>
@@ -4844,8 +5144,11 @@
       <c r="M71" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>187</v>
       </c>
@@ -4881,8 +5184,11 @@
       <c r="M72" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>190</v>
       </c>
@@ -4918,8 +5224,11 @@
       <c r="M73" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>192</v>
       </c>
@@ -4955,8 +5264,11 @@
       <c r="M74" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N74" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>194</v>
       </c>
@@ -4992,8 +5304,11 @@
       <c r="M75" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>196</v>
       </c>
@@ -5029,8 +5344,11 @@
       <c r="M76" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N76" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>198</v>
       </c>
@@ -5066,8 +5384,11 @@
       <c r="M77" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>200</v>
       </c>
@@ -5103,8 +5424,11 @@
       <c r="M78" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N78" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>364075</v>
       </c>
@@ -5140,8 +5464,11 @@
       <c r="M79" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N79" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>201</v>
       </c>
@@ -5177,8 +5504,11 @@
       <c r="M80" s="10" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N80" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>207</v>
       </c>
@@ -5214,8 +5544,11 @@
       <c r="M81" s="10" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N81" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>208</v>
       </c>
@@ -5247,8 +5580,11 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
       <c r="M82" s="10"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N82" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>209</v>
       </c>
@@ -5284,8 +5620,11 @@
       <c r="M83" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N83" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>211</v>
       </c>
@@ -5321,8 +5660,11 @@
       <c r="M84" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N84" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>212</v>
       </c>
@@ -5360,8 +5702,11 @@
       <c r="M85" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N85" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>215</v>
       </c>
@@ -5399,8 +5744,11 @@
       <c r="M86" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N86" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>216</v>
       </c>
@@ -5438,8 +5786,11 @@
       <c r="M87" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N87" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>217</v>
       </c>
@@ -5475,8 +5826,11 @@
       <c r="M88" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N88" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>219</v>
       </c>
@@ -5512,8 +5866,11 @@
       <c r="M89" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N89" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>220</v>
       </c>
@@ -5545,8 +5902,11 @@
       <c r="K90" s="5"/>
       <c r="L90" s="5"/>
       <c r="M90" s="10"/>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N90" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>222</v>
       </c>
@@ -5582,8 +5942,11 @@
       <c r="M91" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N91" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>224</v>
       </c>
@@ -5619,8 +5982,11 @@
       <c r="M92" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N92" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>226</v>
       </c>
@@ -5656,8 +6022,11 @@
       <c r="M93" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N93" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>228</v>
       </c>
@@ -5693,8 +6062,11 @@
       <c r="M94" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N94" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>364073</v>
       </c>
@@ -5730,8 +6102,11 @@
       <c r="M95" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N95" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>230</v>
       </c>
@@ -5767,8 +6142,11 @@
       <c r="M96" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N96" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>231</v>
       </c>
@@ -5804,8 +6182,11 @@
       <c r="M97" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N97" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>235</v>
       </c>
@@ -5841,8 +6222,11 @@
       <c r="M98" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N98" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>237</v>
       </c>
@@ -5876,8 +6260,11 @@
         <v>33</v>
       </c>
       <c r="M99" s="10"/>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N99" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>239</v>
       </c>
@@ -5913,8 +6300,11 @@
       <c r="M100" s="10" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N100" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>242</v>
       </c>
@@ -5952,8 +6342,11 @@
       <c r="M101" s="10" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N101" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>245</v>
       </c>
@@ -5991,8 +6384,11 @@
       <c r="M102" s="10" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N102" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>246</v>
       </c>
@@ -6030,8 +6426,11 @@
       <c r="M103" s="10" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N103" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>247</v>
       </c>
@@ -6063,8 +6462,11 @@
       <c r="K104" s="5"/>
       <c r="L104" s="5"/>
       <c r="M104" s="10"/>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N104" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>248</v>
       </c>
@@ -6100,8 +6502,11 @@
       <c r="M105" s="10" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N105" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
         <v>250</v>
       </c>
@@ -6137,8 +6542,11 @@
       <c r="M106" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N106" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
         <v>252</v>
       </c>
@@ -6174,8 +6582,11 @@
       <c r="M107" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N107" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
         <v>254</v>
       </c>
@@ -6211,8 +6622,11 @@
       <c r="M108" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N108" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>338118</v>
       </c>
@@ -6246,8 +6660,11 @@
         <v>33</v>
       </c>
       <c r="M109" s="10"/>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N109" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>364077</v>
       </c>
@@ -6283,8 +6700,11 @@
       <c r="M110" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N110" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
         <v>257</v>
       </c>
@@ -6320,8 +6740,11 @@
       <c r="M111" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N111" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
         <v>258</v>
       </c>
@@ -6357,8 +6780,11 @@
       <c r="M112" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N112" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
         <v>261</v>
       </c>
@@ -6394,8 +6820,11 @@
       <c r="M113" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N113" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
         <v>262</v>
       </c>
@@ -6429,8 +6858,11 @@
         <v>33</v>
       </c>
       <c r="M114" s="10"/>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N114" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
         <v>359110</v>
       </c>
@@ -6466,8 +6898,11 @@
       <c r="M115" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N115" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
         <v>264</v>
       </c>
@@ -6503,8 +6938,11 @@
       <c r="M116" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N116" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
         <v>266</v>
       </c>
@@ -6540,8 +6978,11 @@
       <c r="M117" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N117" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
         <v>267</v>
       </c>
@@ -6575,8 +7016,11 @@
         <v>33</v>
       </c>
       <c r="M118" s="10"/>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N118" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
         <v>268</v>
       </c>
@@ -6614,8 +7058,11 @@
       <c r="M119" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N119" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
         <v>270</v>
       </c>
@@ -6653,8 +7100,11 @@
       <c r="M120" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N120" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
         <v>271</v>
       </c>
@@ -6692,8 +7142,11 @@
       <c r="M121" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N121" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="8">
         <v>185767</v>
       </c>
@@ -6731,8 +7184,11 @@
       <c r="M122" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N122" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
         <v>185766</v>
       </c>
@@ -6770,8 +7226,11 @@
       <c r="M123" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N123" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
         <v>272</v>
       </c>
@@ -6809,8 +7268,11 @@
       <c r="M124" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N124" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="8">
         <v>364078</v>
       </c>
@@ -6846,8 +7308,11 @@
       <c r="M125" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N125" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
         <v>273</v>
       </c>
@@ -6879,8 +7344,11 @@
       <c r="K126" s="5"/>
       <c r="L126" s="5"/>
       <c r="M126" s="10"/>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N126" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="8">
         <v>364076</v>
       </c>
@@ -6914,8 +7382,11 @@
         <v>33</v>
       </c>
       <c r="M127" s="10"/>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N127" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="s">
         <v>274</v>
       </c>
@@ -6939,8 +7410,11 @@
       <c r="K128" s="5"/>
       <c r="L128" s="5"/>
       <c r="M128" s="10"/>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N128" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
         <v>277</v>
       </c>
@@ -6978,8 +7452,11 @@
       <c r="M129" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N129" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
         <v>279</v>
       </c>
@@ -7017,8 +7494,11 @@
       <c r="M130" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N130" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
         <v>280</v>
       </c>
@@ -7056,8 +7536,11 @@
       <c r="M131" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N131" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>281</v>
       </c>
@@ -7095,8 +7578,11 @@
       <c r="M132" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N132" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
         <v>282</v>
       </c>
@@ -7134,8 +7620,11 @@
       <c r="M133" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N133" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
         <v>283</v>
       </c>
@@ -7173,8 +7662,11 @@
       <c r="M134" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N134" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
         <v>284</v>
       </c>
@@ -7210,8 +7702,11 @@
       <c r="M135" s="10" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N135" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>285</v>
       </c>
@@ -7243,8 +7738,11 @@
       <c r="K136" s="5"/>
       <c r="L136" s="5"/>
       <c r="M136" s="10"/>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N136" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>288</v>
       </c>
@@ -7280,8 +7778,11 @@
       <c r="M137" s="10" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N137" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
         <v>293</v>
       </c>
@@ -7319,8 +7820,11 @@
       <c r="M138" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N138" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
         <v>295</v>
       </c>
@@ -7358,8 +7862,11 @@
       <c r="M139" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N139" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
         <v>296</v>
       </c>
@@ -7397,8 +7904,11 @@
       <c r="M140" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N140" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
         <v>297</v>
       </c>
@@ -7434,8 +7944,11 @@
       <c r="M141" s="10" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N141" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
         <v>301</v>
       </c>
@@ -7467,8 +7980,11 @@
       <c r="K142" s="5"/>
       <c r="L142" s="5"/>
       <c r="M142" s="10"/>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N142" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
         <v>302</v>
       </c>
@@ -7500,8 +8016,11 @@
       <c r="K143" s="5"/>
       <c r="L143" s="5"/>
       <c r="M143" s="10"/>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N143" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
         <v>304</v>
       </c>
@@ -7537,8 +8056,11 @@
       <c r="M144" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N144" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="8">
         <v>147400</v>
       </c>
@@ -7574,8 +8096,11 @@
       <c r="M145" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N145" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>306</v>
       </c>
@@ -7611,8 +8136,11 @@
       <c r="M146" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N146" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="8">
         <v>146918</v>
       </c>
@@ -7648,8 +8176,11 @@
       <c r="M147" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N147" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
         <v>309</v>
       </c>
@@ -7683,8 +8214,11 @@
         <v>33</v>
       </c>
       <c r="M148" s="10"/>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N148" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
         <v>311</v>
       </c>
@@ -7720,8 +8254,11 @@
       <c r="M149" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N149" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="20" t="s">
         <v>353</v>
       </c>
@@ -7737,8 +8274,11 @@
       <c r="K150" s="5"/>
       <c r="L150" s="5"/>
       <c r="M150" s="10"/>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N150" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
         <v>314</v>
       </c>
@@ -7774,8 +8314,11 @@
       <c r="M151" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N151" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>315</v>
       </c>
@@ -7809,8 +8352,11 @@
         <v>33</v>
       </c>
       <c r="M152" s="10"/>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N152" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>319</v>
       </c>
@@ -7848,8 +8394,11 @@
       <c r="M153" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N153" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>321</v>
       </c>
@@ -7887,8 +8436,11 @@
       <c r="M154" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N154" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
         <v>322</v>
       </c>
@@ -7926,8 +8478,11 @@
       <c r="M155" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N155" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>323</v>
       </c>
@@ -7965,8 +8520,11 @@
       <c r="M156" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N156" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="8">
         <v>59572</v>
       </c>
@@ -8004,8 +8562,11 @@
       <c r="M157" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N157" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="8">
         <v>59573</v>
       </c>
@@ -8043,8 +8604,11 @@
       <c r="M158" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N158" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>324</v>
       </c>
@@ -8076,8 +8640,11 @@
       <c r="K159" s="5"/>
       <c r="L159" s="5"/>
       <c r="M159" s="10"/>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N159" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>325</v>
       </c>
@@ -8115,91 +8682,64 @@
       <c r="M160" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A161" s="8" t="s">
+      <c r="N160" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A161" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="B161" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="C161" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D161" s="24"/>
+      <c r="E161" s="25"/>
+      <c r="F161" s="24"/>
+      <c r="G161" s="25"/>
+      <c r="H161" s="24"/>
+      <c r="I161" s="25"/>
+      <c r="J161" s="25"/>
+      <c r="K161" s="25"/>
+      <c r="L161" s="25"/>
+      <c r="M161" s="26"/>
+      <c r="N161" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A162" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="B162" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="C162" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D162" s="24"/>
+      <c r="E162" s="25"/>
+      <c r="F162" s="24"/>
+      <c r="G162" s="25"/>
+      <c r="H162" s="24"/>
+      <c r="I162" s="25"/>
+      <c r="J162" s="25"/>
+      <c r="K162" s="25"/>
+      <c r="L162" s="25"/>
+      <c r="M162" s="26"/>
+      <c r="N162" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A163" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="B161" s="15" t="s">
+      <c r="B163" s="15" t="s">
         <v>330</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D161" s="1"/>
-      <c r="E161" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F161" s="1">
-        <v>50</v>
-      </c>
-      <c r="G161" s="5">
-        <v>50</v>
-      </c>
-      <c r="H161" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I161" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="J161" s="5">
-        <v>2018</v>
-      </c>
-      <c r="K161" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L161" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M161" s="10">
-        <v>65.344999999999999</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A162" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="B162" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D162" s="1"/>
-      <c r="E162" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F162" s="1">
-        <v>25</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="H162" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I162" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="J162" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="K162" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="L162" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M162" s="10">
-        <v>65.344999999999999</v>
-      </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A163" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="B163" s="15" t="s">
-        <v>336</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>29</v>
@@ -8209,22 +8749,22 @@
         <v>47</v>
       </c>
       <c r="F163" s="1">
-        <v>25</v>
-      </c>
-      <c r="G163" s="5" t="s">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="G163" s="5">
+        <v>50</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>162</v>
+        <v>80</v>
       </c>
       <c r="I163" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="J163" s="5" t="s">
-        <v>337</v>
+      <c r="J163" s="5">
+        <v>2018</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>334</v>
+        <v>32</v>
       </c>
       <c r="L163" s="5" t="s">
         <v>33</v>
@@ -8232,35 +8772,38 @@
       <c r="M163" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N163" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="B164" s="15" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D164" s="1"/>
       <c r="E164" s="5" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="F164" s="1">
         <v>25</v>
       </c>
-      <c r="G164" s="5">
-        <v>25</v>
+      <c r="G164" s="5" t="s">
+        <v>332</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>339</v>
+        <v>112</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="K164" s="5" t="s">
         <v>334</v>
@@ -8271,16 +8814,19 @@
       <c r="M164" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N164" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B165" s="15" t="s">
         <v>336</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="5" t="s">
@@ -8293,29 +8839,36 @@
         <v>100</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I165" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J165" s="5">
-        <v>1980</v>
-      </c>
-      <c r="K165" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="J165" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="K165" s="5" t="s">
+        <v>334</v>
+      </c>
       <c r="L165" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M165" s="10"/>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M165" s="10">
+        <v>65.344999999999999</v>
+      </c>
+      <c r="N165" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B166" s="15" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="5" t="s">
@@ -8324,17 +8877,17 @@
       <c r="F166" s="1">
         <v>25</v>
       </c>
-      <c r="G166" s="5" t="s">
-        <v>100</v>
+      <c r="G166" s="5">
+        <v>25</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>162</v>
+        <v>339</v>
       </c>
       <c r="I166" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J166" s="5">
-        <v>1993</v>
+        <v>104</v>
+      </c>
+      <c r="J166" s="5" t="s">
+        <v>340</v>
       </c>
       <c r="K166" s="5" t="s">
         <v>334</v>
@@ -8345,118 +8898,210 @@
       <c r="M166" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N166" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B167" s="15" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="5" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F167" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G167" s="5" t="s">
-        <v>253</v>
+        <v>100</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
       <c r="I167" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J167" s="5">
+        <v>1980</v>
+      </c>
+      <c r="K167" s="5"/>
+      <c r="L167" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M167" s="10"/>
+      <c r="N167" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A168" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B168" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D168" s="1"/>
+      <c r="E168" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F168" s="1">
+        <v>25</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I168" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J167" s="5">
-        <v>2005</v>
-      </c>
-      <c r="K167" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="L167" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M167" s="10">
+      <c r="J168" s="5">
+        <v>1993</v>
+      </c>
+      <c r="K168" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="L168" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M168" s="10">
         <v>65.344999999999999</v>
       </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A168" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="B168" s="16" t="s">
+      <c r="N168" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A169" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="B169" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="C168" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D168" s="13"/>
-      <c r="E168" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F168" s="13">
-        <v>25</v>
-      </c>
-      <c r="G168" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="H168" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="I168" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J168" s="12">
-        <v>1980</v>
-      </c>
-      <c r="K168" s="12"/>
-      <c r="L168" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="M168" s="14"/>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="B169" s="15" t="s">
-        <v>348</v>
-      </c>
       <c r="C169" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D169" s="1"/>
       <c r="E169" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F169" s="1">
+        <v>40</v>
+      </c>
+      <c r="G169" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J169" s="5">
+        <v>2005</v>
+      </c>
+      <c r="K169" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="L169" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M169" s="10">
+        <v>65.344999999999999</v>
+      </c>
+      <c r="N169" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A170" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="B170" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="C170" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D170" s="13"/>
+      <c r="E170" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F169" s="1">
+      <c r="F170" s="13">
         <v>25</v>
       </c>
-      <c r="G169" s="5" t="s">
+      <c r="G170" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="H169" s="1" t="s">
+      <c r="H170" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="I170" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J170" s="12">
+        <v>1980</v>
+      </c>
+      <c r="K170" s="12"/>
+      <c r="L170" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M170" s="14"/>
+      <c r="N170" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B171" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D171" s="1"/>
+      <c r="E171" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F171" s="1">
+        <v>25</v>
+      </c>
+      <c r="G171" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H171" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I169" s="5" t="s">
+      <c r="I171" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="J169" s="5" t="s">
+      <c r="J171" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="K169" s="5" t="s">
+      <c r="K171" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="L169" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M169" s="5">
+      <c r="L171" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M171" s="5">
         <v>65.344999999999999</v>
+      </c>
+      <c r="N171" s="12" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -14734,23 +15379,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100973BFEFB9E8EED45AA48D1DFC8B704A3" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="48fa98e84d6ca432d9ec38d9b25c34f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8208d0d75ea2fc72020bc14120e8df3f" ns3:_="">
     <xsd:import namespace="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
@@ -14932,31 +15560,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB6E9F9-7002-453D-A23F-C770D0B18A16}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C89EA1E5-D714-4CF4-A402-332B720743E2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14972,4 +15593,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12910BB7-EA3B-4F18-8415-6111C589BCB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB6E9F9-7002-453D-A23F-C770D0B18A16}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>